<commit_message>
Updated BOM and partlist
</commit_message>
<xml_diff>
--- a/Electronics/BOM.xlsx
+++ b/Electronics/BOM.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="121">
   <si>
     <t>Number</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>Revision C</t>
+  </si>
+  <si>
+    <t>Non-Ferromagnetic</t>
   </si>
 </sst>
 </file>
@@ -744,13 +747,14 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="118" customWidth="1"/>
   </cols>
   <sheetData>
@@ -948,7 +952,9 @@
         <f t="shared" si="0"/>
         <v>4.6399999999999997</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="H8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1107,7 +1113,9 @@
         <f t="shared" si="0"/>
         <v>13.99</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="H15" s="4" t="s">
         <v>102</v>
       </c>
@@ -1132,7 +1140,9 @@
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="H16" s="4" t="s">
         <v>101</v>
       </c>
@@ -1207,7 +1217,9 @@
         <f t="shared" si="0"/>
         <v>95.97</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="H19" s="4" t="s">
         <v>96</v>
       </c>

</xml_diff>